<commit_message>
excel file rather than txt file
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,6 +742,156 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>vfiizu5d</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange', 'Orange', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[['', 'Red'], ['', 'Blue'], ['', 'Blue'], ['', 'Yellow'], ['', 'Blue'], ['', 'Yellow']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>vfiizu5d</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Purple', 'Orange', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[['', 'Red'], ['', 'Blue'], ['', 'Yellow'], ['', 'Red'], ['', 'Blue'], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>vfiizu5d</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green', 'Purple', 'Orange', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[['', 'Red'], ['', 'Blue'], ['Yellow', ''], ['', 'Red'], ['', 'Blue'], ['', 'Blue']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>vfiizu5d</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple', 'Orange', 'Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[['', 'Red'], ['', 'Blue'], ['', 'Yellow'], ['', 'Red'], ['', 'Blue'], ['', 'Red']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>vfiizu5d</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green', 'Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[['', 'Red'], ['', 'Blue'], ['', 'Yellow'], ['', 'Blue'], ['', 'Red'], ['', 'Red']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>vfiizu5d</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[['', 'Red'], ['', 'Blue'], ['', 'Yellow'], ['', 'Red'], ['', 'Blue'], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
rectangle under the flowers
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="61" customWidth="1" min="4" max="4"/>
-    <col width="95" customWidth="1" min="5" max="5"/>
+    <col width="98" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -892,6 +892,56 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>fsgr7y5o</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange', 'Orange', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', ''], ['Yellow', ''], ['Red', 'Blue'], ['Yellow', ''], ['Blue', 'Red']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fsgr7y5o</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Purple', 'Orange', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Yellow', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
exploration and test 2 added
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="61" customWidth="1" min="4" max="4"/>
     <col width="110" customWidth="1" min="5" max="5"/>
@@ -1242,6 +1242,906 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange', 'Orange', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Purple', 'Orange', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>3</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green', 'Purple', 'Orange', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple', 'Orange', 'Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>5</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green', 'Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Exploration</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Exploration</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Exploration</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>3</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Exploration</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>9vshqapy</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Exploration</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>5</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange', 'Orange', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Purple', 'Orange', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green', 'Purple', 'Orange', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>4</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple', 'Orange', 'Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>5</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green', 'Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>lt530p8m</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Exploration</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Yellow', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>yqlveap5</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange', 'Orange', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>yqlveap5</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>2</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Purple', 'Orange', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>yqlveap5</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>3</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green', 'Purple', 'Orange', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>yqlveap5</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>4</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple', 'Orange', 'Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>yqlveap5</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>5</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green', 'Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>yqlveap5</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange', 'Orange', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Purple', 'Orange', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>3</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green', 'Purple', 'Orange', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple', 'Orange', 'Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>5</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green', 'Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>2</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>3</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>4</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>5</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>cbwk49s2</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert buttons and make them smaller
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2142,6 +2142,206 @@
         </is>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>trbqgy51</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>2</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>3</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>4</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>5</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>koi74k5a</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Change score ; no feedback in transmission ; confirmation for transmitting
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <col width="19" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="61" customWidth="1" min="4" max="4"/>
-    <col width="110" customWidth="1" min="5" max="5"/>
+    <col width="114" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2342,6 +2342,1031 @@
         </is>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>2</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Yellow', 'Red']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>3</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Yellow'], ['Red', 'Blue']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>4</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', 'Yellow']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>5</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', ''], ['Red', 'Yellow']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>[['Yellow', 'Blue'], ['Yellow', 'Yellow'], ['Red', 'Blue'], ['Red', 'Red'], ['Red', 'Yellow'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>2</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>3</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>4</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>5</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>1</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>1</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Blue', ''], ['Blue', ''], ['Blue', ''], ['Red', 'Red']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>1</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>4iaixd9p</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', ''], ['Yellow', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>1</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>2</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>3</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>4</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>5</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Yellow', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>1</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>1</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>2</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>3</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>4</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>5</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>5virtmb4</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>1</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>gtot06qe</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>1</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>gtot06qe</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>2</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>gtot06qe</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>3</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>gtot06qe</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>4</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>gtot06qe</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>5</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>gtot06qe</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>[['Yellow', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
modification next round button
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +767,2256 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>41esdihg</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>41esdihg</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>dujujdf2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>dujujdf2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>dujujdf2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>dujujdf2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>dujujdf2</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>5</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>f1n5lvu1</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>5</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>5</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>5</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>5m2a8s1h</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>4</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ozekcq01</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>5</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>3</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Yellow', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>5</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>2</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>5</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>xiujz7jc</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>2</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>3</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>5</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>2</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>3</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>4</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>5</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>7omxd8wq</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>wr0q4nhq</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>wr0q4nhq</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>2</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>wr0q4nhq</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>3</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>wr0q4nhq</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>4</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>wr0q4nhq</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>5</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>1</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>1</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>a9zqtjgv</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>1</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>1</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>2</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>3</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>4</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>5</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>1</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>2</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>3</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>4</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>5</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>s2yrbcq7</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>1</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
alligner les slots et pas les fleurs
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaag\OneDrive\Bureau\Scolarite depuis prepa\2025-2026\Projet\Otree_Flower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533BC617-1056-4498-96C4-065E450CA5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3B718B-D3A0-498A-B86A-DED6750CBF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
modified between phases buttons
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaag\OneDrive\Bureau\Scolarite depuis prepa\2025-2026\Projet\Otree_Flower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA876C48-BC5A-4CCF-ADE5-E418BA326520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D9339D-5E5A-435E-8BD2-E860D8096574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,7 +668,7 @@
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="56" customWidth="1"/>
     <col min="6" max="6" width="114" customWidth="1"/>
-    <col min="7" max="7" width="64" customWidth="1"/>
+    <col min="7" max="7" width="38" customWidth="1"/>
     <col min="8" max="8" width="185" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
total earnings in excel
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaag\OneDrive\Bureau\Scolarite depuis prepa\2025-2026\Projet\Otree_Flower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D9339D-5E5A-435E-8BD2-E860D8096574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F5847E-7629-4915-B72B-F2EDF9C90ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="107">
   <si>
     <t>Treatment</t>
   </si>
@@ -46,6 +46,9 @@
     <t>noise_effects</t>
   </si>
   <si>
+    <t>final_total_earnings</t>
+  </si>
+  <si>
     <t>Anomaly no noise</t>
   </si>
   <si>
@@ -293,6 +296,51 @@
   </si>
   <si>
     <t>[None, None, {'index': 2, 'type': 'decrease', 'amount': -0.2, 'before': 1.0, 'after': 0.8}, None, {'index': 4, 'type': 'decrease', 'amount': -0.2, 'before': 1.0, 'after': 0.8}, None]</t>
+  </si>
+  <si>
+    <t>vk4huyhx</t>
+  </si>
+  <si>
+    <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+  </si>
+  <si>
+    <t>[0.25, 0.25, 0.25]</t>
+  </si>
+  <si>
+    <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+  </si>
+  <si>
+    <t>[0.25, 0.5, 0.5]</t>
+  </si>
+  <si>
+    <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+  </si>
+  <si>
+    <t>[0.5, 0.5, 0.5]</t>
+  </si>
+  <si>
+    <t>[['Blue', ''], ['Red', ''], ['Red', '']]</t>
+  </si>
+  <si>
+    <t>[0.5, 0.25, 0.25]</t>
+  </si>
+  <si>
+    <t>[['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+  </si>
+  <si>
+    <t>[0.25, 0.25, 0.25, 0.25, 0.25, 0.25]</t>
+  </si>
+  <si>
+    <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+  </si>
+  <si>
+    <t>[0.25, 0.5, 0.25]</t>
+  </si>
+  <si>
+    <t>[['Blue', ''], ['Blue', ''], ['Red', '']]</t>
+  </si>
+  <si>
+    <t>[0.5, 0.5, 0.25]</t>
   </si>
 </sst>
 </file>
@@ -655,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,9 +718,10 @@
     <col min="6" max="6" width="114" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
     <col min="8" max="8" width="185" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,1253 +746,1583 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
-        <v>37</v>
-      </c>
       <c r="H11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="I13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="H14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D24">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="I25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
         <v>74</v>
       </c>
-      <c r="G27" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D30">
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D36">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="I37">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" t="s">
-        <v>79</v>
-      </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D41">
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D42">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" t="s">
-        <v>79</v>
-      </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D46">
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H46" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F47" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G47" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H48" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" t="s">
+        <v>90</v>
+      </c>
+      <c r="H49" t="s">
+        <v>91</v>
+      </c>
+      <c r="I49">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" t="s">
+        <v>94</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
+      </c>
+      <c r="G51" t="s">
+        <v>96</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>97</v>
+      </c>
+      <c r="G52" t="s">
+        <v>98</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" t="s">
+        <v>99</v>
+      </c>
+      <c r="G53" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" t="s">
+        <v>99</v>
+      </c>
+      <c r="G54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" t="s">
         <v>28</v>
       </c>
-      <c r="F49" t="s">
-        <v>88</v>
-      </c>
-      <c r="G49" t="s">
-        <v>89</v>
-      </c>
-      <c r="H49" t="s">
-        <v>90</v>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" t="s">
+        <v>102</v>
+      </c>
+      <c r="H55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" t="s">
+        <v>93</v>
+      </c>
+      <c r="G57" t="s">
+        <v>94</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>39</v>
+      </c>
+      <c r="F58" t="s">
+        <v>103</v>
+      </c>
+      <c r="G58" t="s">
+        <v>104</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>39</v>
+      </c>
+      <c r="F59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59" t="s">
+        <v>106</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>39</v>
+      </c>
+      <c r="F60" t="s">
+        <v>93</v>
+      </c>
+      <c r="G60" t="s">
+        <v>94</v>
+      </c>
+      <c r="H60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" t="s">
+        <v>101</v>
+      </c>
+      <c r="G61" t="s">
+        <v>102</v>
+      </c>
+      <c r="H61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
growth min to 0.3
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaag\OneDrive\Bureau\Scolarite depuis prepa\2025-2026\Projet\Otree_Flower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829BF786-CF9F-4F20-B2C6-203123C9BC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F39901-1F7F-4CDB-9CC7-DCF420CB7272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,7 +660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
replace nutrients by dragging on top
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaag\OneDrive\Bureau\Scolarite depuis prepa\2025-2026\Projet\Otree_Flower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F39901-1F7F-4CDB-9CC7-DCF420CB7272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A0590A-89FE-43AE-91AA-67D2BE803565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
create transmission treatments add popup transmission
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
@@ -2916,6 +2916,291 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>3</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>5</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Blue'], ['Blue', 'Blue'], ['Blue', 'Blue'], ['Blue', 'Blue'], ['Blue', 'Blue'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>yp80d4yg</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Yellow'], ['Yellow', 'Yellow'], ['Red', 'Blue'], ['Red', 'Red'], ['Yellow', 'Red'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add see combination throughout exp
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3201,6 +3201,716 @@
         </is>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>8l60xdc4</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>['5', '5', '5']</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Transmission M&amp;M</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>zkjjaoa6</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>['5', '5', '5']</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>ygg4hk51</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Transmission M&amp;M</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>bh4i5uou</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>['2', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Transmission M&amp;M</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>94uigg6z</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>8qiqijij</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>8qiqijij</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Transmission M&amp;M</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>7tfvji4f</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>['2', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>vf3wsvvg</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>['2', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>x7c4pnjr</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Red', ''], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>['8', '2', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>x7c4pnjr</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>['2', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>xcowwowp</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>['8', '10', '2']</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Transmission M&amp;M</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>lssyg1wd</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue'], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>['8', '10', '5']</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>M&amp;M no noise</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>8khfl1x3</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>['10', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Anomaly noisy</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>va0caf9s</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>[None, None, {'index': 2, 'type': 'increase', 'amount': 0.2, 'before': 0.25, 'after': 0.45}]</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>['8', '10', '4']</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>M&amp;M noisy</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>sm0rfajc</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>[None, {'index': 1, 'type': 'decrease', 'amount': -0.2, 'before': 0.5, 'after': 0.3}, None]</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>['10', '3', '3']</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
modify No Anomaly treatment and flower sets
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3911,6 +3911,1661 @@
         </is>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>k1rmtlii</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>[['Yellow', 'Red'], ['Blue', 'Red'], ['Blue', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>['6', '8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>k1rmtlii</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>2</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>['2', '5', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>k1rmtlii</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Yellow'], ['Red', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>['8', '8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>k1rmtlii</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>4</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Blue'], ['Red', 'Red'], ['Yellow', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>['10', '5', '6']</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>k1rmtlii</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>5</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>['Green', 'Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Yellow'], ['Yellow', 'Red'], ['Red', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>['8', '6', '8']</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>0.98</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>76to9fji</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>nf0a674u</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>['7', '3']</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>76to9fji</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>2</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>76to9fji</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>['2', '5', '5']</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ixvai9kk</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>de2py1lo</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>de2py1lo</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>de2py1lo</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>3</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>['2', '5', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>de2py1lo</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>4</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>['2', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>wabfo7n0</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>wabfo7n0</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>wabfo7n0</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>3</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>['2', '2', '5']</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>98bygjmo</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>98bygjmo</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>2</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>98bygjmo</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>3</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>['2', '5', '3']</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>y6fnfhf9</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>['7', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>y6fnfhf9</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>2</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>['3', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>y6fnfhf9</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>3</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>['7', '7', '7']</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>dcgogwtg</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>['7', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>dcgogwtg</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>2</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>['Green', 'Green', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>['7', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>dcgogwtg</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>3</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>['10', '7', '7']</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>5s99x6kc</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>['Purple', 'Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>['8', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>5s99x6kc</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>2</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>['8', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>5s99x6kc</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>3</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>['5', '5', '5']</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>['10', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>2</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Yellow', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>['7', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>3</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', 'Yellow'], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>['7', '10', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>4</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', ''], ['Yellow', '']]</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>['7', '7', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Yellow', ''], ['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>['Orange', 'Orange']</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>['7', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>2</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', 'Red']]</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>['7', '7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>3</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>['Red', 'Blue', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>['6', '6', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>4</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>['7', '7', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>5</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>['Purple', 'Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>['7', '7', '3']</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>jhpkpf1h</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', ''], ['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify all the treatments and scorings to match
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5566,6 +5566,706 @@
         </is>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>mni5vgdn</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>1</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Red'], ['Blue', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>mni5vgdn</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>2</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>[['Yellow', 'Blue'], ['Blue', 'Red']]</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>2</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Yellow'], ['Red', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>3</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>['2', '5', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>mni5vgdn</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>3</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>['2', '5', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>4</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>mni5vgdn</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>4</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>No Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>mni5vgdn</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>['2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>2</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>['2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>3</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>['Green', 'Red', 'Green']</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>['2', '5', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>4</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>['Blue', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>['2', '5', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>i6vtqbf9</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>5</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>['5', '2', '2']</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>0.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>No Anomaly noisy</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>anucg6jd</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>1</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>[{'index': 0, 'type': 'increase', 'amount': 0.2, 'before': 0.5, 'after': 0.7}, None]</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>['7', '10']</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Anomaly noisy</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>tbcsissw</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>[None, {'index': 1, 'type': 'decrease', 'amount': -0.2, 'before': 1.0, 'after': 0.8}]</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>['5', '8']</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify the transmission treatments accordingly
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6266,6 +6266,136 @@
         </is>
       </c>
     </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>e0y4cjuz</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>e0y4cjuz</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>2</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Transmission M&amp;M</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>c2lm5k76</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>1</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
change flowers design and sequence
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4681,6 +4681,586 @@
         </is>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>['8', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>['8', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Blue'], ['Blue', 'Red']]</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>['10', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>['8', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Red'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>['8', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>[['Blue', 'Blue'], ['Red', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>['10', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>cn0o2558</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>2</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>['8', '10']</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>htd2mqsv</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>htd2mqsv</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>['2', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>htd2mqsv</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>2</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>[['Red', 'Red'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>['5', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>htd2mqsv</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>3</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Yellow', 'Yellow'], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>['2', '6', '10']</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>htd2mqsv</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>4</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', 'Blue']]</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>['2', '5', '10']</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>vde2r9iw</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>e6k1fezv</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify background, all white
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5261,6 +5261,91 @@
         </is>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>uhl6f983</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>uhl6f983</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>2</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
change the showing of the transmission
</commit_message>
<xml_diff>
--- a/nutrient_flower_data.xlsx
+++ b/nutrient_flower_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5346,6 +5346,541 @@
         </is>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Anomaly no noise</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>yxuau6po</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>[['Red', 'Blue'], ['Blue', 'Yellow']]</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>['8', '8']</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>2nj8y4ca</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green']</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>2</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>['2', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>3</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Green']</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>['2', '5', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Training phase</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>4</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>['Green', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>[['Blue', ''], ['Blue', ''], ['Blue', '']]</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>['5', '5', '5']</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Blue', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>1</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>['Orange', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>['2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>2</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>['Orange', 'Green']</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>[None, None]</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>['2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>3</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>['Green', 'Red', 'Green']</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>4</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>['Blue', 'Purple', 'Purple']</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Exploration phase</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>5</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>['Purple', 'Green', 'Yellow']</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>[None, None, None]</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>['2', '2', '2']</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Transmission correct</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>txpcyowh</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>['Green', 'Yellow', 'Purple', 'Red', 'Orange', 'Blue']</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>[['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', ''], ['Red', '']]</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>[None, None, None, None, None, None]</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>['0', '0', '0', '0', '0', '0']</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>0.67</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>